<commit_message>
Change 'Europees Parlementsverkiezingen' to 'Europese Parlementsverkiezingen'
</commit_message>
<xml_diff>
--- a/files/Stembureaus Open Data Standaard 1.4 - Provinciale Statenverkiezingen 2023 voorbeeld.xlsx
+++ b/files/Stembureaus Open Data Standaard 1.4 - Provinciale Statenverkiezingen 2023 voorbeeld.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="174">
   <si>
     <t xml:space="preserve">Toelichting</t>
   </si>
@@ -100,24 +100,11 @@
 – Deze versie is voor het eerst te gebruiken voor de gemeenteraadsverkiezingen van 16 maart 2022.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Versie 1.4:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">– ‘Leesloep’ verwijderd uit de voorbeelden van het ‘Visuele hulpmiddelen’-attribuut.</t>
-    </r>
+    <t xml:space="preserve">Versie 1.4:
+– ‘Leesloep’ verwijderd uit de voorbeelden van het ‘Visuele hulpmiddelen’-attribuut.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">– Aanpassen van ‘Europees Parlementsverkiezingen’ naar ‘Europese Parlementsverkiezing’.</t>
   </si>
   <si>
     <t xml:space="preserve">Verplicht (ja/nee)</t>
@@ -363,25 +350,7 @@
     <t xml:space="preserve">Visuele hulpmiddelen</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Welke visuele hulpmiddelen zijn aanwezig? Dit is een vrij tekstveld.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> NB: een leesloep is verplicht op elk stembureau en moet hier dus niet vermeld worden.</t>
-    </r>
+    <t xml:space="preserve">Welke visuele hulpmiddelen zijn aanwezig? Dit is een vrij tekstveld. NB: een leesloep is verplicht op elk stembureau en moet hier dus niet vermeld worden.</t>
   </si>
   <si>
     <t xml:space="preserve">stemmal, vrijwilliger/host aanwezig</t>
@@ -403,7 +372,7 @@
 – Gemeenteraadsverkiezingen: kieskring is gemeentenaam
 – Eilandsraadsverkiezingen: kieskring is eilandnaam
 – Kiescollegeverkiezingen: kieskring is eilandnaam
-– Europees Parlementsverkiezingen: kieskring is 'Nederland'
+– Europese Parlementsverkiezingen: kieskring is 'Nederland'
 – Waterschapsverkiezingen: kieskring is waterschapsnaam</t>
   </si>
   <si>
@@ -419,7 +388,7 @@
 – Gemeenteraadsverkiezingen: gemeente
 – Eilandsraadsverkiezingen: eiland
 – Kiescollegeverkiezingen: eiland
-– Europees Parlementsverkiezing: Nederland
+– Europese Parlementsverkiezingen: Nederland
 – Waterschapsverkiezingen: waterschap</t>
   </si>
   <si>
@@ -473,7 +442,7 @@
     <t xml:space="preserve">Titel</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;verkiezing&gt;: keuze uit 'Tweede Kamerverkiezingen', 'gemeenteraadsverkiezingen', 'Provinciale Statenverkiezingen', 'referendum &lt;naam van referendum&gt;', 'eilandsraadsverkiezingen', 'kiescollegeverkiezingen', 'Europees Parlementsverkiezingen', 'waterschapsverkiezingen', 'verkiezingen gebiedscommissies en wijkraden' en 'verkiezingen stadsdeelcommissies'
+    <t xml:space="preserve">&lt;verkiezing&gt;: keuze uit 'Tweede Kamerverkiezingen', 'gemeenteraadsverkiezingen', 'Provinciale Statenverkiezingen', 'referendum &lt;naam van referendum&gt;', 'eilandsraadsverkiezingen', 'kiescollegeverkiezingen', 'Europese Parlementsverkiezingen', 'waterschapsverkiezingen', 'verkiezingen gebiedscommissies en wijkraden' en 'verkiezingen stadsdeelcommissies'
 &lt;jaar&gt;: het jaar waarin de verkiezing wordt gehouden; dit moet weggelaten worden bij referenda aangezien de titel per referendum anders is</t>
   </si>
   <si>
@@ -500,7 +469,7 @@
     <t xml:space="preserve">Omschrijving</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;verkiezing&gt;: keuze uit 'de Tweede Kamerverkiezingen', 'de gemeenteraadsverkiezingen', 'de Provinciale Statenverkiezingen', 'referendum &lt;naam van referendum&gt;', 'de kiescollegeverkiezingen', 'de eilandsraadsverkiezingen', 'de Europees Parlementsverkiezingen', 'de waterschapsverkiezingen', 'verkiezingen gebiedscommissies en wijkraden' en 'verkiezingen stadsdeelcommissies'
+    <t xml:space="preserve">&lt;verkiezing&gt;: keuze uit 'de Tweede Kamerverkiezingen', 'de gemeenteraadsverkiezingen', 'de Provinciale Statenverkiezingen', 'referendum &lt;naam van referendum&gt;', 'de kiescollegeverkiezingen', 'de eilandsraadsverkiezingen', 'de Europese Parlementsverkiezingen', 'de waterschapsverkiezingen', 'verkiezingen gebiedscommissies en wijkraden' en 'verkiezingen stadsdeelcommissies'
 &lt;datum&gt;: in format zoals '16 maart 2022'</t>
   </si>
   <si>
@@ -540,7 +509,7 @@
     <t xml:space="preserve">Tags</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;aard van de verkiezing&gt;: keuze uit 'Tweede Kamerverkiezingen', 'gemeenteraadsverkiezingen', 'Provinciale Statenverkiezingen', 'referendum', 'eilandsraadsverkiezingen', 'kiescollegeverkiezingen', 'Europees Parlementsverkiezingen', 'waterschapsverkiezingen', 'verkiezingen gebiedscommissies en wijkraden' en 'verkiezingen stadsdeelcommissies'</t>
+    <t xml:space="preserve">&lt;aard van de verkiezing&gt;: keuze uit 'Tweede Kamerverkiezingen', 'gemeenteraadsverkiezingen', 'Provinciale Statenverkiezingen', 'referendum', 'eilandsraadsverkiezingen', 'kiescollegeverkiezingen', 'Europese Parlementsverkiezingen', 'waterschapsverkiezingen', 'verkiezingen gebiedscommissies en wijkraden' en 'verkiezingen stadsdeelcommissies'</t>
   </si>
   <si>
     <t xml:space="preserve">verkiezingen, stembureaus, overheid, democratie, stemmen, kiesdistrict, &lt;aard van de verkiezing&gt;</t>
@@ -565,7 +534,7 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;gebied&gt;: afhankelijk van de verkiezing, keuze uit
-– 'Nederland' voor Tweede Kamerverkiezingen, Europees Parlementsverkiezingen en referendum
+– 'Nederland' voor Tweede Kamerverkiezingen, Europese Parlementsverkiezingen en referendum
 – 'Europees Nederland' voor gemeenteraadsverkiezingen, Provinciale Statenverkiezingen, waterschapsverkiezingen en referendum
 – 'Caribisch Nederland' voor eilandsraadsverkiezingen, kiescollegeverkiezingen en referendum
 – &lt;de namen van de gemeenten&gt; in het geval van gemeenteraadsverkiezingen bij een herindeling
@@ -676,7 +645,7 @@
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -745,6 +714,15 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -753,15 +731,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -822,11 +791,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -868,12 +832,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u val="single"/>
@@ -1006,7 +964,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1058,18 +1016,21 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1078,9 +1039,6 @@
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
@@ -1123,22 +1081,22 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="11" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="11" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -1159,19 +1117,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="12" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="12" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="12" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="12" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1187,15 +1145,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1211,7 +1169,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1219,7 +1177,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1239,7 +1197,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1255,19 +1213,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1275,11 +1233,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="12" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="12" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1343,7 +1301,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1371,14 +1329,14 @@
     <cellStyle name="Footnote 9" xfId="34"/>
     <cellStyle name="Good 12" xfId="35"/>
     <cellStyle name="Good 13" xfId="36"/>
-    <cellStyle name="Heading 1 5" xfId="37"/>
-    <cellStyle name="Heading 1 6" xfId="38"/>
-    <cellStyle name="Heading 2 6" xfId="39"/>
-    <cellStyle name="Heading 2 7" xfId="40"/>
-    <cellStyle name="Heading 3" xfId="41"/>
-    <cellStyle name="Heading 4" xfId="42"/>
-    <cellStyle name="Heading 5" xfId="43"/>
-    <cellStyle name="Heading 1" xfId="44"/>
+    <cellStyle name="Heading 1 1" xfId="37"/>
+    <cellStyle name="Heading 1 5" xfId="38"/>
+    <cellStyle name="Heading 1 6" xfId="39"/>
+    <cellStyle name="Heading 2 6" xfId="40"/>
+    <cellStyle name="Heading 2 7" xfId="41"/>
+    <cellStyle name="Heading 3" xfId="42"/>
+    <cellStyle name="Heading 4" xfId="43"/>
+    <cellStyle name="Heading 5" xfId="44"/>
     <cellStyle name="Hyperlink 10" xfId="45"/>
     <cellStyle name="Hyperlink 11" xfId="46"/>
     <cellStyle name="Neutral 13" xfId="47"/>
@@ -1469,7 +1427,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1542,6 +1500,11 @@
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1568,7 +1531,7 @@
       <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="36.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="19.22"/>
@@ -1587,16 +1550,16 @@
         <v>2</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="9"/>
@@ -1631,19 +1594,19 @@
     </row>
     <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="8"/>
@@ -1659,21 +1622,21 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -1688,18 +1651,18 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4" s="14" t="n">
         <v>517</v>
@@ -1720,17 +1683,17 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="8"/>
@@ -1746,21 +1709,21 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="8"/>
@@ -1778,19 +1741,19 @@
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="8"/>
@@ -1808,15 +1771,15 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="8"/>
@@ -1834,15 +1797,15 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="8"/>
@@ -1860,15 +1823,15 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="8"/>
@@ -1886,15 +1849,15 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="8"/>
@@ -1910,21 +1873,21 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="8"/>
@@ -1942,15 +1905,15 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="12"/>
       <c r="E13" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="8"/>
@@ -1968,10 +1931,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="12"/>
@@ -1994,10 +1957,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="12"/>
@@ -2018,10 +1981,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="12"/>
@@ -2042,17 +2005,17 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="8"/>
@@ -2070,15 +2033,15 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="12"/>
       <c r="E18" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F18" s="15"/>
       <c r="G18" s="8"/>
@@ -2094,21 +2057,21 @@
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="8"/>
@@ -2124,18 +2087,18 @@
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E20" s="18" t="n">
         <v>81611</v>
@@ -2154,18 +2117,18 @@
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
     </row>
-    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E21" s="18" t="n">
         <v>454909</v>
@@ -2184,18 +2147,18 @@
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E22" s="18" t="n">
         <v>52.0775912</v>
@@ -2214,18 +2177,18 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="13" t="s">
         <v>74</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>73</v>
       </c>
       <c r="E23" s="18" t="n">
         <v>4.3166395</v>
@@ -2244,21 +2207,21 @@
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F24" s="26"/>
       <c r="G24" s="8"/>
@@ -2274,21 +2237,21 @@
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
@@ -2302,21 +2265,21 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>82</v>
-      </c>
       <c r="E26" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F26" s="15"/>
       <c r="G26" s="8"/>
@@ -2334,19 +2297,19 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="8"/>
@@ -2364,19 +2327,19 @@
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F28" s="15"/>
       <c r="G28" s="8"/>
@@ -2394,19 +2357,19 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
@@ -2424,16 +2387,16 @@
     </row>
     <row r="30" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E30" s="27" t="n">
         <v>1</v>
@@ -2452,21 +2415,21 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F31" s="15"/>
       <c r="G31" s="8"/>
@@ -2484,19 +2447,19 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F32" s="15"/>
       <c r="G32" s="8"/>
@@ -2512,21 +2475,21 @@
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
     </row>
-    <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="28" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F33" s="15"/>
       <c r="G33" s="8"/>
@@ -2542,21 +2505,21 @@
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
     </row>
-    <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="28" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E34" s="31" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F34" s="32"/>
       <c r="G34" s="8"/>
@@ -2572,21 +2535,21 @@
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
     </row>
-    <row r="35" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="17" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F35" s="32"/>
       <c r="G35" s="8"/>
@@ -2663,16 +2626,16 @@
         <v>4</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -2680,21 +2643,21 @@
       <c r="I1" s="36"/>
       <c r="J1" s="8"/>
     </row>
-    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="37" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -2712,37 +2675,37 @@
     </row>
     <row r="3" s="4" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="40" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -2760,19 +2723,19 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="40" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D5" s="43" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="8"/>
@@ -2790,19 +2753,19 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="40" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D6" s="44" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="44" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -2818,21 +2781,21 @@
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
     </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="40" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B7" s="41" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D7" s="44" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -2850,19 +2813,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="40" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D8" s="44" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" s="44" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -2878,21 +2841,21 @@
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
     </row>
-    <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="40" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="8"/>
@@ -2910,17 +2873,17 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="40" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D10" s="44"/>
       <c r="E10" s="44" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
@@ -2938,17 +2901,17 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="40" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D11" s="44"/>
       <c r="E11" s="44" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F11" s="39"/>
       <c r="G11" s="8"/>
@@ -2964,21 +2927,21 @@
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
     </row>
-    <row r="12" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="40" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="8"/>
@@ -2996,19 +2959,19 @@
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="40" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E13" s="45" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
@@ -3026,17 +2989,17 @@
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="40" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B14" s="41" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D14" s="46"/>
       <c r="E14" s="46" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="1"/>
@@ -3054,19 +3017,19 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="40" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E15" s="47" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="1"/>
@@ -3084,19 +3047,19 @@
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="40" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
@@ -3114,19 +3077,19 @@
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="40" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E17" s="45" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
@@ -3144,17 +3107,17 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C18" s="42" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D18" s="49"/>
       <c r="E18" s="49" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F18" s="39"/>
       <c r="G18" s="8"/>
@@ -3172,17 +3135,17 @@
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="40" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D19" s="46"/>
       <c r="E19" s="43" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="1"/>
@@ -3200,19 +3163,19 @@
     </row>
     <row r="20" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="40" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
@@ -3230,16 +3193,16 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="28" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C21" s="50" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update URLs of Rijksoverheid regarding a11y during elections; Some changes to the Stembureaus ODS: don't allow 'nee' etc. for some fields, add two a11y fields, change some form texts
</commit_message>
<xml_diff>
--- a/files/Stembureaus Open Data Standaard 1.4 - Provinciale Statenverkiezingen 2023 voorbeeld.xlsx
+++ b/files/Stembureaus Open Data Standaard 1.4 - Provinciale Statenverkiezingen 2023 voorbeeld.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="183">
   <si>
     <t xml:space="preserve">Toelichting</t>
   </si>
@@ -100,11 +100,83 @@
 – Deze versie is voor het eerst te gebruiken voor de gemeenteraadsverkiezingen van 16 maart 2022.</t>
   </si>
   <si>
-    <t xml:space="preserve">Versie 1.4:
-– ‘Leesloep’ verwijderd uit de voorbeelden van het ‘Visuele hulpmiddelen’-attribuut.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">– Aanpassen van ‘Europees Parlementsverkiezingen’ naar ‘Europese Parlementsverkiezing’.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Versie 1.4:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">– </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Toevoeging van ‘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Toegankelijke ov-halte’-attribuut.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">– Toevoeging van ‘Extra toegankelijkheidsinformatie’-attribuut.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">– ‘schrijftolk’ toegevoegd aan de voorbeelden van het ‘Auditieve hulpmiddelen’-attribuut.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">– ‘leesloep’ verwijderd uit de voorbeelden van het ‘Visuele hulpmiddelen’-attribuut.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">– ‘soundbox’ en ‘geleidelijnen’ toegevoegd aan de voorbeelden van het ‘Visuele hulpmiddelen’-attribuut.
+– Aan de beschrijvingen van ‘Extra adresinformatie’-, ‘Auditieve hulpmiddelen‘- en ‘Visuele hulpmiddelen’-attributen toegevoegd dat het veld leeg gelaten moet worden als het antwoord ‘nee’ is.
+– Aanpassen van ‘Europees Parlementsverkiezingen’ naar ‘Europese Parlementsverkiezing’.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Verplicht (ja/nee)</t>
@@ -266,6 +338,9 @@
 Caribisch Nederland (BES-eilanden) vult verplicht hier het hele adres in.</t>
   </si>
   <si>
+    <t xml:space="preserve">tekst; als er geen extra informatie is, laat dit veld dan leeg (‘nee’ e.d. worden automatisch verwijderd)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ingang aan achterkant gebouw</t>
   </si>
   <si>
@@ -325,10 +400,40 @@
   <si>
     <t xml:space="preserve">Is het stembureau toegankelijk voor mensen met een lichamelijke beperking?
 Voor meer informatie, zie:
-https://www.rijksoverheid.nl/documenten/publicaties/2021/10/14/toegankelijkheid-verkiezingen</t>
+https://www.rijksoverheid.nl/onderwerpen/verkiezingen/verkiezingentoolkit/toegankelijkheid-verkiezingen</t>
   </si>
   <si>
     <t xml:space="preserve">ja of nee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toegankelijke ov-halte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is er een toegankelijke ov-halte in de buurt? Beschrijf hoe ver deze van het stembureau ligt en hoe deze toegankelijk is.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tekst</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">; als er geen toegankelijke ov-halte is, laat dit veld dan leeg (‘nee’ e.d. worden automatisch verwijderd)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">binnen 100 meter, rolstoeltoegankelijk, geleidelijnen</t>
   </si>
   <si>
     <t xml:space="preserve">Akoestiek</t>
@@ -341,25 +446,56 @@
     <t xml:space="preserve">Auditieve hulpmiddelen</t>
   </si>
   <si>
-    <t xml:space="preserve">Welke auditieve hulpmiddelen zijn aanwezig? Dit is een vrij tekstveld.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gebarentolk</t>
+    <t xml:space="preserve">Welke auditieve hulpmiddelen voor slechthorende en doven zijn aanwezig? Dit is een vrij tekstveld.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tekst; als er geen hulpmiddelen zijn, laat dit veld dan leeg (‘nee’ e.d. worden automatisch verwijderd).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gebarentolk, schrijftolk</t>
   </si>
   <si>
     <t xml:space="preserve">Visuele hulpmiddelen</t>
   </si>
   <si>
-    <t xml:space="preserve">Welke visuele hulpmiddelen zijn aanwezig? Dit is een vrij tekstveld. NB: een leesloep is verplicht op elk stembureau en moet hier dus niet vermeld worden.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stemmal, vrijwilliger/host aanwezig</t>
+    <t xml:space="preserve">Welke visuele hulpmiddelen voor blinden en slechtzienden zijn aanwezig? Dit is een vrij tekstveld.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tekst; als er geen hulpmiddelen zijn, laat dit veld dan leeg (‘nee’ e.d. worden automatisch verwijderd). NB: een leesloep is verplicht op elk stembureau en moet hier dus niet vermeld worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stemmal, soundbox, vrijwilliger/host aanwezig, geleidelijnen</t>
   </si>
   <si>
     <t xml:space="preserve">Gehandicaptentoilet</t>
   </si>
   <si>
     <t xml:space="preserve">Is er een gehandicaptentoilet aanwezig? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra toegankelijkheidsinformatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eventuele extra informatie over de toegankelijkheid van dit stembureau.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">prikkelarm stembureau, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">stembureau is volledig toegankelijk voor mensen met een lichamelijke beperking er is echter geen gehandicaptenparkeerplaats</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Kieskring ID</t>
@@ -645,7 +781,7 @@
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -791,10 +927,21 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -964,7 +1111,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1081,26 +1228,26 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="11" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="11" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1117,19 +1264,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="12" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="12" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="12" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="12" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1145,15 +1292,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1169,7 +1316,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1177,7 +1324,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1197,35 +1344,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1233,11 +1388,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="12" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="12" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1301,7 +1456,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1427,7 +1582,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1497,14 +1652,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1523,7 +1673,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AMJ39"/>
+  <dimension ref="A1:AMJ41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -1550,16 +1700,16 @@
         <v>2</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="9"/>
@@ -1594,19 +1744,19 @@
     </row>
     <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="14" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>21</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="8"/>
@@ -1624,19 +1774,19 @@
     </row>
     <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="16" t="s">
         <v>25</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>26</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -1653,16 +1803,16 @@
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>28</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>29</v>
       </c>
       <c r="E4" s="14" t="n">
         <v>517</v>
@@ -1683,17 +1833,17 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="8"/>
@@ -1711,19 +1861,19 @@
     </row>
     <row r="6" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="13" t="s">
+      <c r="D6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>34</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>35</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="8"/>
@@ -1741,19 +1891,19 @@
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="E7" s="18" t="s">
         <v>38</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>39</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="8"/>
@@ -1771,15 +1921,15 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="8"/>
@@ -1797,15 +1947,15 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="8"/>
@@ -1823,15 +1973,15 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="8"/>
@@ -1849,15 +1999,15 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="8"/>
@@ -1875,19 +2025,19 @@
     </row>
     <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="13" t="s">
+      <c r="D12" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="22" t="s">
         <v>49</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>50</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="8"/>
@@ -1905,15 +2055,15 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="12"/>
       <c r="E13" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="8"/>
@@ -1931,10 +2081,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="12"/>
@@ -1957,10 +2107,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="12"/>
@@ -1981,10 +2131,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="12"/>
@@ -2005,17 +2155,17 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="18" t="s">
         <v>57</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>58</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="8"/>
@@ -2033,15 +2183,15 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="12"/>
       <c r="E18" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F18" s="15"/>
       <c r="G18" s="8"/>
@@ -2059,18 +2209,18 @@
     </row>
     <row r="19" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="C19" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="D19" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="25" t="s">
         <v>64</v>
       </c>
       <c r="F19" s="15"/>
@@ -2092,7 +2242,7 @@
         <v>65</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>66</v>
@@ -2122,7 +2272,7 @@
         <v>68</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>69</v>
@@ -2212,7 +2362,7 @@
         <v>77</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>78</v>
@@ -2220,10 +2370,10 @@
       <c r="D24" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="F24" s="26"/>
+      <c r="F24" s="27"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
@@ -2242,7 +2392,7 @@
         <v>81</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>82</v>
@@ -2251,7 +2401,7 @@
         <v>83</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
@@ -2266,24 +2416,22 @@
       <c r="R25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="11" t="s">
         <v>84</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="12" t="s">
-        <v>83</v>
+      <c r="D26" s="19" t="s">
+        <v>86</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" s="15"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="23"/>
+        <v>87</v>
+      </c>
+      <c r="H26" s="8"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
@@ -2295,21 +2443,21 @@
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="17" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="8"/>
@@ -2327,19 +2475,19 @@
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>92</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F28" s="15"/>
       <c r="G28" s="8"/>
@@ -2355,23 +2503,23 @@
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="17" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>83</v>
+        <v>17</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>96</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" s="8"/>
+        <v>97</v>
+      </c>
+      <c r="F29" s="15"/>
       <c r="G29" s="8"/>
       <c r="H29" s="23"/>
       <c r="I29" s="8"/>
@@ -2385,23 +2533,23 @@
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
     </row>
-    <row r="30" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="17" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E30" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F30" s="15"/>
+        <v>17</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="H30" s="23"/>
       <c r="I30" s="8"/>
@@ -2415,25 +2563,25 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="17" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E31" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="F31" s="15"/>
+        <v>17</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="F31" s="8"/>
       <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
+      <c r="H31" s="23"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
@@ -2445,25 +2593,25 @@
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="17" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="E32" s="27" t="s">
-        <v>23</v>
+        <v>104</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="E32" s="29" t="n">
+        <v>1</v>
       </c>
       <c r="F32" s="15"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
+      <c r="H32" s="23"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
@@ -2475,21 +2623,21 @@
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
     </row>
-    <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="B33" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="E33" s="30" t="s">
-        <v>105</v>
+    <row r="33" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>108</v>
       </c>
       <c r="F33" s="15"/>
       <c r="G33" s="8"/>
@@ -2505,25 +2653,25 @@
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
     </row>
-    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="B34" s="29" t="s">
-        <v>23</v>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E34" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="F34" s="32"/>
+        <v>110</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F34" s="15"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="23"/>
+      <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
@@ -2535,25 +2683,25 @@
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
     </row>
-    <row r="35" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="D35" s="1" t="s">
+    <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="E35" s="18" t="s">
+      <c r="B35" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="F35" s="32"/>
+      <c r="D35" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E35" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="F35" s="15"/>
       <c r="G35" s="8"/>
-      <c r="H35" s="23"/>
+      <c r="H35" s="8"/>
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
@@ -2565,26 +2713,86 @@
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="13"/>
-      <c r="B36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="33"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13"/>
-      <c r="B37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="33"/>
+    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="F36" s="34"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+    </row>
+    <row r="37" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="F37" s="34"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="13"/>
       <c r="B38" s="12"/>
       <c r="D38" s="12"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
+      <c r="E38" s="35"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F39" s="33"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="35"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F41" s="35"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2612,52 +2820,52 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="19.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="29" width="17.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="29" width="70.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="29" width="79.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="29" width="69.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="29" width="75.87"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="29" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="19.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="17.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="31" width="70.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="31" width="79.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="31" width="69.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="31" width="75.87"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="31" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="36"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="38"/>
       <c r="J1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>114</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>115</v>
+      <c r="A2" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>124</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -2674,38 +2882,38 @@
       <c r="R2" s="8"/>
     </row>
     <row r="3" s="4" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>18</v>
+      <c r="A3" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>17</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>120</v>
+        <v>128</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>129</v>
       </c>
       <c r="H3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="40" t="s">
-        <v>121</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>23</v>
+      <c r="A4" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D4" s="35" t="s">
-        <v>123</v>
+        <v>131</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>132</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -2722,20 +2930,20 @@
       <c r="R4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="40" t="s">
-        <v>125</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="D5" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="43" t="s">
-        <v>127</v>
+      <c r="A5" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>136</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="8"/>
@@ -2752,20 +2960,20 @@
       <c r="R5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="40" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="D6" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="44" t="s">
-        <v>129</v>
+      <c r="A6" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="46" t="s">
+        <v>138</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -2782,20 +2990,20 @@
       <c r="R6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="40" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="D7" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="44" t="s">
-        <v>131</v>
+      <c r="A7" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>140</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -2812,20 +3020,20 @@
       <c r="R7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="44" t="s">
-        <v>133</v>
+      <c r="A8" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="D8" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>142</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -2842,20 +3050,20 @@
       <c r="R8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>18</v>
+      <c r="A9" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D9" s="35" t="s">
-        <v>136</v>
+        <v>144</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>145</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="8"/>
@@ -2872,18 +3080,18 @@
       <c r="R9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="40" t="s">
-        <v>138</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44" t="s">
-        <v>139</v>
+      <c r="A10" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46" t="s">
+        <v>148</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
@@ -2900,20 +3108,20 @@
       <c r="R10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="40" t="s">
-        <v>140</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="F11" s="39"/>
+      <c r="A11" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" s="41"/>
       <c r="G11" s="8"/>
       <c r="H11" s="1"/>
       <c r="I11" s="8"/>
@@ -2928,20 +3136,20 @@
       <c r="R11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="40" t="s">
-        <v>142</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="D12" s="35" t="s">
-        <v>144</v>
+      <c r="A12" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>153</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="8"/>
@@ -2958,20 +3166,20 @@
       <c r="R12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>147</v>
-      </c>
-      <c r="D13" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="E13" s="45" t="s">
-        <v>149</v>
+      <c r="A13" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="E13" s="47" t="s">
+        <v>158</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
@@ -2988,18 +3196,18 @@
       <c r="R13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="B14" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46" t="s">
-        <v>151</v>
+      <c r="A14" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="B14" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48" t="s">
+        <v>160</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="1"/>
@@ -3016,24 +3224,24 @@
       <c r="R14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="40" t="s">
-        <v>152</v>
-      </c>
-      <c r="B15" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="35" t="s">
-        <v>153</v>
-      </c>
-      <c r="D15" s="35" t="s">
-        <v>154</v>
-      </c>
-      <c r="E15" s="47" t="s">
-        <v>155</v>
+      <c r="A15" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="D15" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="E15" s="49" t="s">
+        <v>164</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="48"/>
+      <c r="H15" s="50"/>
       <c r="I15" s="8"/>
       <c r="J15" s="1"/>
       <c r="K15" s="8"/>
@@ -3046,24 +3254,24 @@
       <c r="R15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="B16" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="35" t="s">
-        <v>157</v>
-      </c>
-      <c r="D16" s="32" t="s">
-        <v>158</v>
-      </c>
-      <c r="E16" s="32" t="s">
-        <v>159</v>
+      <c r="A16" s="42" t="s">
+        <v>165</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>168</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
-      <c r="H16" s="48"/>
+      <c r="H16" s="50"/>
       <c r="I16" s="8"/>
       <c r="J16" s="1"/>
       <c r="K16" s="8"/>
@@ -3076,24 +3284,24 @@
       <c r="R16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="40" t="s">
-        <v>160</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="35" t="s">
-        <v>161</v>
-      </c>
-      <c r="D17" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="E17" s="45" t="s">
-        <v>149</v>
+      <c r="A17" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="E17" s="47" t="s">
+        <v>158</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
-      <c r="H17" s="48"/>
+      <c r="H17" s="50"/>
       <c r="I17" s="8"/>
       <c r="J17" s="1"/>
       <c r="K17" s="8"/>
@@ -3106,22 +3314,22 @@
       <c r="R17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="B18" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49" t="s">
-        <v>163</v>
-      </c>
-      <c r="F18" s="39"/>
+      <c r="A18" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51" t="s">
+        <v>172</v>
+      </c>
+      <c r="F18" s="41"/>
       <c r="G18" s="8"/>
-      <c r="H18" s="48"/>
+      <c r="H18" s="50"/>
       <c r="I18" s="8"/>
       <c r="J18" s="1"/>
       <c r="K18" s="8"/>
@@ -3134,18 +3342,18 @@
       <c r="R18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="B19" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="42" t="s">
-        <v>165</v>
-      </c>
-      <c r="D19" s="46"/>
-      <c r="E19" s="43" t="s">
-        <v>166</v>
+      <c r="A19" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="B19" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="D19" s="48"/>
+      <c r="E19" s="45" t="s">
+        <v>175</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="1"/>
@@ -3162,20 +3370,20 @@
       <c r="R19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="40" t="s">
-        <v>167</v>
-      </c>
-      <c r="B20" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="35" t="s">
-        <v>168</v>
+      <c r="A20" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="B20" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>177</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
@@ -3192,17 +3400,17 @@
       <c r="R20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="50" t="s">
-        <v>172</v>
-      </c>
-      <c r="E21" s="29" t="s">
-        <v>173</v>
+      <c r="A21" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="52" t="s">
+        <v>181</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update standard: removed information about stembureaus met beperkte toegang from "Extra adresaanduiding", no longer relevant
</commit_message>
<xml_diff>
--- a/files/Stembureaus Open Data Standaard 1.4 - Provinciale Statenverkiezingen 2023 voorbeeld.xlsx
+++ b/files/Stembureaus Open Data Standaard 1.4 - Provinciale Statenverkiezingen 2023 voorbeeld.xlsx
@@ -189,7 +189,8 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">– Toevoeging van ‘Type stembureau’-attribuut.
-– Opmerking toegevoegd aan ‘Bag Nummeraanduiding ID’-attribuut over de benodigde opmaak van de cel.</t>
+– Opmerking toegevoegd aan ‘Bag Nummeraanduiding ID’-attribuut over de benodigde opmaak van de cel.
+– Informatie over stembureaus met beperkte toegang weggehaald uit ‘Extra adresaanduiding’-attribuut aangezien dit niet meer van toepassing is.</t>
     </r>
   </si>
   <si>
@@ -409,7 +410,6 @@
   </si>
   <si>
     <t xml:space="preserve">Eventuele extra informatie over de locatie van het stembureau. Bv. 'Ingang aan achterkant gebouw' of 'Mobiel stembureau op het midden van het plein'.
-Sommige stembureaus zijn niet open voor algemeen publiek vanwege coronamaatregelen. Bijvoorbeeld een stembureau in een verzorgingshuis. Geef dat in dit veld aan door exact de tekst 'Niet open voor algemeen publiek' in te voeren.
 Caribisch Nederland (BES-eilanden) vult verplicht hier het hele adres in.</t>
   </si>
   <si>
@@ -1796,7 +1796,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
         <v>13</v>
       </c>
@@ -2400,7 +2400,7 @@
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
Big update for 2023 elections: remove/comment code relevant only to the previous elections (gemeenteraadsverkiezingen 2022); apply changes for Stembureau Open Data Standaard v1.4 (adds fields "Type stembureau", "Toegankelijke ov-halte", "Extra toegankelijkheidsinformatie" and splits "Openingstijden" into "Openingstijd" and "Sluitingstijd" + textual/info changes); change elections from 2022GR to 2023PS/WS/ER/KC; update gemeenten; some fixes
</commit_message>
<xml_diff>
--- a/files/Stembureaus Open Data Standaard 1.4 - Provinciale Statenverkiezingen 2023 voorbeeld.xlsx
+++ b/files/Stembureaus Open Data Standaard 1.4 - Provinciale Statenverkiezingen 2023 voorbeeld.xlsx
@@ -63,6 +63,7 @@
         <sz val="10"/>
         <rFont val="arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">informatie over het opslaan van data volgens deze standaard in CSV-, spreadsheet- en JSON-bestandsformaten.</t>
     </r>
@@ -180,194 +181,149 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">– Opmerking toegevoegd dat stembureaus die op meerdere dagen open zijn voor elke dag een ander stembureau nummer moeten hebben en dus apart moeten worden ingevoerd.
+– Toevoeging van ‘Type stembureau’-attribuut.
+– Opmerking toegevoegd aan ‘Bag Nummeraanduiding ID’-attribuut over de benodigde opmaak van de cel.
+– Informatie over stembureaus met beperkte toegang weggehaald uit ‘Extra adresaanduiding’-attribuut aangezien dit niet meer van toepassing is.
 </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">– Toevoeging van ‘Type stembureau’-attribuut.
-– Opmerking toegevoegd aan ‘Bag Nummeraanduiding ID’-attribuut over de benodigde opmaak van de cel.
-– Informatie over stembureaus met beperkte toegang weggehaald uit ‘Extra adresaanduiding’-attribuut aangezien dit niet meer van toepassing is.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Verplicht (ja/nee)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Opmerkingen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Format</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voorbeeld</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gemeente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CBS gemeentenaam, zie https://opendata.cbs.nl/statline/#/CBS/nl/dataset/85067NED/table?dl=B165 of gebruik Bonaire, Sint Eustatius of Saba.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tekst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'s-Gravenhage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CBS gemeentecode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CBS gemeentecode bestaande uit 6 karakters, zie https://opendata.cbs.nl/statline/#/CBS/nl/dataset/85067NED/table?dl=B165 of gebruik GM9001 voor Bonaire, GM9002 voor Sint Eustatius of GM9003 voor Saba. Deze methode wordt gehanteerd totdat TOOI operationeel is voor verwijzing.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GM&lt;4 cijfers&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GM0518</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nummer stembureau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Een stembureau is gevestigd in een stemlokaal en elk stembureau heeft een eigen nummer. Sommige stemlokalen hebben meerdere stembureaus. Elk stembureau moet apart ingevoerd worden ook al is de locatie (het stemlokaal) hetzelfde aangezien elk stembureau een ander nummer heeft.
-Als een stembureau meerdere dagen open is dan moet deze voor elke dag een ander stembureaunummer hebben. Elke stembureau(nummer) moet dus apart ingevoerd worden.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cijfers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Naam stembureau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stadhuis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type stembureau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;type&gt;: keuze uit 'regulier', ‘bijzonder’ en ‘mobiel’.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;type&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regulier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gebruiksdoel van het gebouw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gebruiksdoel van het gebouw waar het stembureau huist volgens de BAG.
-Voor uitgebreidere beschrijving van bovenstaande gebruiksdoelen zie: https://www.amsterdam.nl/stelselpedia/bag-index/handboek-inwinnen/introductie-bag/registratie/gebruiksdoel/
-Gebruiksdoel van elk gebouw is te vinden door het adres op https://bagviewer.kadaster.nl/ in te voeren en rechts onder het kopje 'Verblijfsobject' te kijken.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">keuze uit: 'Wonen', 'Bijeenkomst', 'Winkel', 'Gezondheidszorg', 'Kantoor', 'Logies', 'Industrie', 'Onderwijs', 'Sport', 'Overig', 'Cel'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kantoor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Website locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Website van de locatie van het stembureau, indien aanwezig; Een URL moet met 'http://' of 'https://' beginnen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">URL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.denhaag.nl/nl/bestuur-en-organisatie/contact-met-de-gemeente/stadhuis-den-haag.htm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wijknaam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Centrum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CBS Wijknummer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WK051828</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buurtnaam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kortenbos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CBS Buurtnummer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BU05182811</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAG Nummeraanduiding ID</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">BAG Nummeraanduiding ID, vindbaar door het adres van het stembureau op https://bagviewer.kadaster.nl/ in te voeren en rechts onder het kopje 'Nummeraanduiding' te kijken.
+      <t xml:space="preserve">– URL van CBS-tabel met gemeentenamen en -codes aangepast naar de 2023 versie.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Verplicht (ja/nee)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opmerkingen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voorbeeld</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gemeente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CBS gemeentenaam, zie https://opendata.cbs.nl/statline/#/CBS/nl/dataset/85067NED/table?dl=B165 of gebruik Bonaire, Sint Eustatius of Saba.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tekst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'s-Gravenhage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CBS gemeentecode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CBS gemeentecode bestaande uit 6 karakters, zie https://opendata.cbs.nl/statline/#/CBS/nl/dataset/85067NED/table?dl=B165 of gebruik GM9001 voor Bonaire, GM9002 voor Sint Eustatius of GM9003 voor Saba. Deze methode wordt gehanteerd totdat TOOI operationeel is voor verwijzing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GM&lt;4 cijfers&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GM0518</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nummer stembureau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Een stembureau is gevestigd in een stemlokaal en elk stembureau heeft een eigen nummer. Sommige stemlokalen hebben meerdere stembureaus. Elk stembureau moet apart ingevoerd worden ook al is de locatie (het stemlokaal) hetzelfde aangezien elk stembureau een ander nummer heeft.
+Als een stembureau meerdere dagen open is dan moet deze voor elke dag een ander stembureaunummer hebben. Elk stembureau(nummer) moet dus apart ingevoerd worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cijfers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naam stembureau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stadhuis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type stembureau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kies ‘regulier’ als dit een normaal stembureau betreft. Kies ‘bijzonder’ als het stembureau afwijkende openingstijden heeft. Kies ‘mobiel’ als het stembureau meerdere locaties heeft.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keuze uit 'regulier', ‘bijzonder’ en ‘mobiel’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regulier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gebruiksdoel van het gebouw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gebruiksdoel van het gebouw waar het stembureau huist volgens de BAG.
+Voor uitgebreidere beschrijving van bovenstaande gebruiksdoelen zie: https://www.amsterdam.nl/stelselpedia/bag-index/handboek-inwinnen/introductie-bag/registratie/gebruiksdoel/
+Gebruiksdoel van elk gebouw is te vinden door het adres op https://bagviewer.kadaster.nl/ in te voeren en rechts onder het kopje 'Verblijfsobject' te kijken.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keuze uit: 'Wonen', 'Bijeenkomst', 'Winkel', 'Gezondheidszorg', 'Kantoor', 'Logies', 'Industrie', 'Onderwijs', 'Sport', 'Overig', 'Cel'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kantoor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website locatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website van de locatie van het stembureau, indien aanwezig; Een URL moet met 'http://' of 'https://' beginnen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.denhaag.nl/nl/bestuur-en-organisatie/contact-met-de-gemeente/stadhuis-den-haag.htm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wijknaam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CBS Wijknummer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WK051828</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buurtnaam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kortenbos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CBS Buurtnummer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BU05182811</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG Nummeraanduiding ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG Nummeraanduiding ID, vindbaar door het adres van het stembureau op https://bagviewer.kadaster.nl/ in te voeren en rechts onder het kopje 'Nummeraanduiding' te kijken.
 Wordt de ID niet goed opgeslagen? Zorg dan dat de cel opgemaakt is als ‘tekst’ of plaats voor de ID één aanhalingsteken (').
-Vermeld voor mobiele stembureaus die vlakbij een gebouw staan of locaties zonder BAG Nummeraanduiding ID het BAG Nummeraanduiding ID van het </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">dichtstbijzijnde gebouw</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> en gebruik eventueel het 'Extra adresaanduiding'-veld om de locatie van stembureau te beschrijven. Mocht een (mobiel) stembureau niet in de buurt van een gebouw staan, voer dan </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">'0000000000000000' (zestien keer het getal '0') in; 'Extra adresaanduiding'-attribuut is dan verplicht. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">NB: de precieze locatie geeft u aan met de 'Latitude' en 'Longitude'-velden.
+Vermeld voor mobiele stembureaus die vlakbij een gebouw staan of locaties zonder BAG Nummeraanduiding ID het BAG Nummeraanduiding ID van het dichtstbijzijnde gebouw en gebruik eventueel het 'Extra adresaanduiding'-veld om de locatie van stembureau te beschrijven. Mocht een (mobiel) stembureau niet in de buurt van een gebouw staan, voer dan '0000000000000000' (zestien keer het getal '0') in; 'Extra adresaanduiding'-attribuut is dan verplicht. NB: de precieze locatie geeft u aan met de 'Latitude' en 'Longitude'-velden.
 Caribisch Nederland (BES-eilanden) staat niet in de BAG. Deze gemeenten moeten '0000000000000000' (zestien keer het getal '0') invullen en het adres verplicht invullen in het 'Extra adresaanduiding'-attribuut.</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">0518200000747446</t>
@@ -466,13 +422,13 @@
     <t xml:space="preserve">YYYY-MM-DDTHH:MM:SS</t>
   </si>
   <si>
-    <t xml:space="preserve">2022-03-16T07:30:00</t>
+    <t xml:space="preserve">2023-03-15T07:30:00</t>
   </si>
   <si>
     <t xml:space="preserve">Sluitingstijd</t>
   </si>
   <si>
-    <t xml:space="preserve">2022-03-16T21:00:00</t>
+    <t xml:space="preserve">2023-03-15T21:00:00</t>
   </si>
   <si>
     <t xml:space="preserve">Toegankelijk voor mensen met een lichamelijke beperking</t>
@@ -631,13 +587,13 @@
     <t xml:space="preserve">Stembureaus &lt;verkiezing&gt; &lt;jaar&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Stembureaus gemeenteraadsverkiezingen 2022</t>
+    <t xml:space="preserve">Stembureaus Provinciale Statenverkiezingen 2023</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;CBS gemeentecode&gt;: code bestaande uit 6 karakters, zie https://opendata.cbs.nl/statline/#/CBS/nl/dataset/85067NED/table?dl=B165 of gebruik GM9001 voor Bonaire, GM9002 voor Sint Eustatius of GM9003 voor Saba.
+    <t xml:space="preserve">&lt;CBS gemeentecode&gt;: code bestaande uit 6 karakters, zie https://opendata.cbs.nl/#/CBS/nl/dataset/85385NED/table?dl=B165 of gebruik GM9001 voor Bonaire, GM9002 voor Sint Eustatius of GM9003 voor Saba.
 &lt;YYYYMMDD&gt;: datum van de verkiezing
 &lt;oplopend getal&gt;: getal tussen 000 en 999</t>
   </si>
@@ -645,20 +601,20 @@
     <t xml:space="preserve">NLODS&lt;CBS gemeentecode&gt;stembureaus&lt;YYYYMMDD&gt;&lt;oplopend getal van 000 t/m 999&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">NLODSGM0518stembureaus20220316009</t>
+    <t xml:space="preserve">NLODSGM0518stembureaus20230315010</t>
   </si>
   <si>
     <t xml:space="preserve">Omschrijving</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;verkiezing&gt;: keuze uit 'de Tweede Kamerverkiezingen', 'de gemeenteraadsverkiezingen', 'de Provinciale Statenverkiezingen', 'referendum &lt;naam van referendum&gt;', 'de kiescollegeverkiezingen', 'de eilandsraadsverkiezingen', 'de Europese Parlementsverkiezingen', 'de waterschapsverkiezingen', 'verkiezingen gebiedscommissies en wijkraden' en 'verkiezingen stadsdeelcommissies'
-&lt;datum&gt;: in format zoals '16 maart 2022'</t>
+&lt;datum&gt;: in format zoals '15 maart 2023'</t>
   </si>
   <si>
     <t xml:space="preserve">Overzicht van de locaties van stembureaus. De gegevens hebben betrekking op &lt;verkiezing&gt; op &lt;datum&gt;.</t>
   </si>
   <si>
-    <t xml:space="preserve">Overzicht van de locaties van stembureaus. De gegevens hebben betrekking op de gemeenteraadsverkiezingen op 16 maart 2022.</t>
+    <t xml:space="preserve">Overzicht van de locaties van stembureaus. De gegevens hebben betrekking op de Provinciale Statenverkiezingen op 15 maart 2023.</t>
   </si>
   <si>
     <t xml:space="preserve">Eigenaar</t>
@@ -738,7 +694,7 @@
     <t xml:space="preserve">YYYY-MM-DDTHH:MM:SS+-HH:MM</t>
   </si>
   <si>
-    <t xml:space="preserve">2022-01-16T13:05:23+01:00</t>
+    <t xml:space="preserve">2023-01-16T13:05:23+01:00</t>
   </si>
   <si>
     <t xml:space="preserve">Relatie / gebruik andere standaarden</t>
@@ -756,19 +712,19 @@
     <t xml:space="preserve">YYYY-MM-DD</t>
   </si>
   <si>
-    <t xml:space="preserve">2022-03-16</t>
+    <t xml:space="preserve">2023-03-15</t>
   </si>
   <si>
     <t xml:space="preserve">Update frequentie</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;datum verkiezing&gt;: in format zoals '16 maart 2022'</t>
+    <t xml:space="preserve">&lt;datum verkiezing&gt;: in format zoals '15 maart 2023'</t>
   </si>
   <si>
     <t xml:space="preserve">Incidenteel tot en met &lt;datum verkiezing&gt; (uiterste bekendmaking van stembureaus is 4 dagen voor de verkiezing)</t>
   </si>
   <si>
-    <t xml:space="preserve">Incidenteel tot en met 16 maart 2022 (uiterste bekendmaking van stembureaus is 4 dagen voor de verkiezingen)</t>
+    <t xml:space="preserve">Incidenteel tot en met 15 maart 2023 (uiterste bekendmaking van stembureaus is 4 dagen voor de verkiezingen)</t>
   </si>
   <si>
     <t xml:space="preserve">Wijzigings datum</t>
@@ -844,10 +800,10 @@
             "Latitude": 51.34711,
             "Longitude": 5.45515,
             "Openingstijden": [
-                {"Openingstijd": "2022-03-15T10:00:00", "Sluitingstijd": "2022-03-15T13:00:00"},
-                {"Openingstijd": "2022-03-15T14:00:00", "Sluitingstijd": "2022-03-15T21:00:00"},
-                {"Openingstijd": "2022-03-16T10:00:00", "Sluitingstijd": "2022-03-15T13:00:00"},
-                {"Openingstijd": "2022-03-16T14:00:00", "Sluitingstijd": "2022-03-15T21:00:00"},
+                {"Openingstijd": "2023-03-14T10:00:00", "Sluitingstijd": "2023-03-14T13:00:00"},
+                {"Openingstijd": "2023-03-14T14:00:00", "Sluitingstijd": "2023-03-14T21:00:00"},
+                {"Openingstijd": "2023-03-15T10:00:00", "Sluitingstijd": "2023-03-15T13:00:00"},
+                {"Openingstijd": "2023-03-15T14:00:00", "Sluitingstijd": "2023-03-15T21:00:00"},
                 ... 
             ]   
             "Toegankelijk voor mensen met een lichamelijke beperking": "ja",
@@ -864,7 +820,7 @@
     "Contactgegevens gemeente": "verkiezingen@valkenswaard.nl",
     "Verkiezingswebsite gemeente": "http://www.valkenswaard.nl/verkiezingen",
     "Verkiezingen": '', 
-    "ID": "NLODSGM0858stembureaus20220316009"
+    "ID": "NLODSGM0858stembureaus20230315010"
   },  
   ... 
 ]</t>
@@ -879,7 +835,7 @@
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1027,11 +983,6 @@
       <sz val="10"/>
       <name val="arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="arial"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1077,12 +1028,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1229,7 +1174,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1346,22 +1291,22 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="11" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="11" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -1382,215 +1327,215 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="12" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="12" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="60" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="12" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="12" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="12" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="60" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="12" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1796,7 +1741,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
         <v>13</v>
       </c>
@@ -2003,7 +1948,7 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" s="23" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="23" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
         <v>33</v>
       </c>
@@ -3658,9 +3603,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="129.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="129.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>